<commit_message>
adding legend fix issues'
</commit_message>
<xml_diff>
--- a/data_summary.xlsx
+++ b/data_summary.xlsx
@@ -518,7 +518,7 @@
         <v>9.23</v>
       </c>
       <c r="C2" t="n">
-        <v>19.86000061035156</v>
+        <v>19.93000030517578</v>
       </c>
       <c r="D2" t="n">
         <v>20.01</v>
@@ -527,7 +527,7 @@
         <v>10.77</v>
       </c>
       <c r="F2" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="G2" t="n">
         <v>0.05</v>
@@ -536,7 +536,7 @@
         <v>0.6</v>
       </c>
       <c r="I2" t="n">
-        <v>0.25</v>
+        <v>0.239999994635582</v>
       </c>
       <c r="J2" t="n">
         <v>0.1</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>19.86±0.24</t>
+          <t>19.93±0.22</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -560,7 +560,7 @@
         <v>-3.08</v>
       </c>
       <c r="O2" t="n">
-        <v>84.59</v>
+        <v>87.67</v>
       </c>
       <c r="P2" t="n">
         <v>118.34</v>
@@ -574,7 +574,7 @@
         <v>17.65</v>
       </c>
       <c r="C3" t="n">
-        <v>25.39999961853027</v>
+        <v>25.29000091552734</v>
       </c>
       <c r="D3" t="n">
         <v>25.05</v>
@@ -583,7 +583,7 @@
         <v>7.35</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="G3" t="n">
         <v>0.23</v>
@@ -604,7 +604,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>25.4±0.22</t>
+          <t>25.29±0.22</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -616,7 +616,7 @@
         <v>17.47</v>
       </c>
       <c r="O3" t="n">
-        <v>80.26000000000001</v>
+        <v>84.61</v>
       </c>
       <c r="P3" t="n">
         <v>91.52</v>
@@ -630,7 +630,7 @@
         <v>25.1</v>
       </c>
       <c r="C4" t="n">
-        <v>30.19000053405762</v>
+        <v>30.09000015258789</v>
       </c>
       <c r="D4" t="n">
         <v>29.97</v>
@@ -639,7 +639,7 @@
         <v>4.9</v>
       </c>
       <c r="F4" t="n">
-        <v>0.19</v>
+        <v>0.11</v>
       </c>
       <c r="G4" t="n">
         <v>0.19</v>
@@ -660,7 +660,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>30.19±0.1</t>
+          <t>30.09±0.1</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -672,7 +672,7 @@
         <v>32.61</v>
       </c>
       <c r="O4" t="n">
-        <v>98.52</v>
+        <v>106.83</v>
       </c>
       <c r="P4" t="n">
         <v>99.12</v>
@@ -686,7 +686,7 @@
         <v>27.65</v>
       </c>
       <c r="C5" t="n">
-        <v>31.79999923706055</v>
+        <v>31.70999908447266</v>
       </c>
       <c r="D5" t="n">
         <v>31.88</v>
@@ -695,7 +695,7 @@
         <v>4.35</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.29</v>
       </c>
       <c r="G5" t="n">
         <v>0.15</v>
@@ -716,7 +716,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>31.8±0.12</t>
+          <t>31.71±0.12</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -728,7 +728,7 @@
         <v>36.85</v>
       </c>
       <c r="O5" t="n">
-        <v>96.26000000000001</v>
+        <v>91.41</v>
       </c>
       <c r="P5" t="n">
         <v>102.92</v>
@@ -742,7 +742,7 @@
         <v>32.6</v>
       </c>
       <c r="C6" t="n">
-        <v>34.93000030517578</v>
+        <v>34.88000106811523</v>
       </c>
       <c r="D6" t="n">
         <v>34.86</v>
@@ -751,7 +751,7 @@
         <v>2.4</v>
       </c>
       <c r="F6" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="G6" t="n">
         <v>0.16</v>
@@ -772,7 +772,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>34.93±0.1</t>
+          <t>34.88±0.1</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -784,7 +784,7 @@
         <v>51.82</v>
       </c>
       <c r="O6" t="n">
-        <v>112.07</v>
+        <v>107.65</v>
       </c>
       <c r="P6" t="n">
         <v>103.26</v>
@@ -798,7 +798,7 @@
         <v>36.21</v>
       </c>
       <c r="C7" t="n">
-        <v>37.20000076293945</v>
+        <v>37.16999816894531</v>
       </c>
       <c r="D7" t="n">
         <v>36.89</v>
@@ -807,7 +807,7 @@
         <v>0.82</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="G7" t="n">
         <v>0.16</v>
@@ -816,7 +816,7 @@
         <v>0.46</v>
       </c>
       <c r="I7" t="n">
-        <v>0.09000000357627869</v>
+        <v>0.1000000014901161</v>
       </c>
       <c r="J7" t="n">
         <v>0.18</v>
@@ -828,7 +828,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>37.2±0.09</t>
+          <t>37.17±0.09</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -840,7 +840,7 @@
         <v>73.59999999999999</v>
       </c>
       <c r="O7" t="n">
-        <v>102.59</v>
+        <v>104.74</v>
       </c>
       <c r="P7" t="n">
         <v>104.42</v>
@@ -854,7 +854,7 @@
         <v>40.59</v>
       </c>
       <c r="C8" t="n">
-        <v>39.95000076293945</v>
+        <v>39.93999862670898</v>
       </c>
       <c r="D8" t="n">
         <v>39.89</v>
@@ -884,7 +884,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>39.95±0.08</t>
+          <t>39.94±0.08</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -896,7 +896,7 @@
         <v>79.93000000000001</v>
       </c>
       <c r="O8" t="n">
-        <v>116.17</v>
+        <v>115.33</v>
       </c>
       <c r="P8" t="n">
         <v>105.61</v>
@@ -910,7 +910,7 @@
         <v>45.5</v>
       </c>
       <c r="C9" t="n">
-        <v>43.02999877929688</v>
+        <v>43.02000045776367</v>
       </c>
       <c r="D9" t="n">
         <v>42.9</v>
@@ -940,7 +940,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>43.03±0.1</t>
+          <t>43.02±0.1</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -952,7 +952,7 @@
         <v>57.6</v>
       </c>
       <c r="O9" t="n">
-        <v>114.86</v>
+        <v>115.02</v>
       </c>
       <c r="P9" t="n">
         <v>108.87</v>
@@ -966,7 +966,7 @@
         <v>48.75</v>
       </c>
       <c r="C10" t="n">
-        <v>45.06000137329102</v>
+        <v>45.04999923706055</v>
       </c>
       <c r="D10" t="n">
         <v>44.8</v>
@@ -996,7 +996,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>45.06±0.19</t>
+          <t>45.05±0.19</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1008,7 +1008,7 @@
         <v>51.08</v>
       </c>
       <c r="O10" t="n">
-        <v>105.3</v>
+        <v>105.55</v>
       </c>
       <c r="P10" t="n">
         <v>107.44</v>
@@ -1022,7 +1022,7 @@
         <v>51.9</v>
       </c>
       <c r="C11" t="n">
-        <v>47.04000091552734</v>
+        <v>47.02999877929688</v>
       </c>
       <c r="D11" t="n">
         <v>46.77</v>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>47.04±0.16</t>
+          <t>47.03±0.16</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1064,7 +1064,7 @@
         <v>47.14</v>
       </c>
       <c r="O11" t="n">
-        <v>110.04</v>
+        <v>110.41</v>
       </c>
       <c r="P11" t="n">
         <v>105.94</v>
@@ -1078,7 +1078,7 @@
         <v>61.49</v>
       </c>
       <c r="C12" t="n">
-        <v>53.13999938964844</v>
+        <v>53.09999847412109</v>
       </c>
       <c r="D12" t="n">
         <v>52.74</v>
@@ -1087,7 +1087,7 @@
         <v>8.49</v>
       </c>
       <c r="F12" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="G12" t="n">
         <v>0.17</v>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>53.14±0.17</t>
+          <t>53.1±0.17</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1120,7 +1120,7 @@
         <v>39.56</v>
       </c>
       <c r="O12" t="n">
-        <v>106.49</v>
+        <v>107.92</v>
       </c>
       <c r="P12" t="n">
         <v>110.45</v>
@@ -1134,7 +1134,7 @@
         <v>64.54000000000001</v>
       </c>
       <c r="C13" t="n">
-        <v>55.11000061035156</v>
+        <v>55.06999969482422</v>
       </c>
       <c r="D13" t="n">
         <v>54.72</v>
@@ -1143,7 +1143,7 @@
         <v>9.539999999999999</v>
       </c>
       <c r="F13" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="G13" t="n">
         <v>0.26</v>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>55.11±0.15</t>
+          <t>55.07±0.15</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1176,7 +1176,7 @@
         <v>38.2</v>
       </c>
       <c r="O13" t="n">
-        <v>111.86</v>
+        <v>113.7</v>
       </c>
       <c r="P13" t="n">
         <v>105.68</v>
@@ -1190,7 +1190,7 @@
         <v>67.22</v>
       </c>
       <c r="C14" t="n">
-        <v>56.83000183105469</v>
+        <v>56.79000091552734</v>
       </c>
       <c r="D14" t="n">
         <v>56.69</v>
@@ -1199,7 +1199,7 @@
         <v>10.22</v>
       </c>
       <c r="F14" t="n">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="G14" t="n">
         <v>0.33</v>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>56.83±0.21</t>
+          <t>56.79±0.21</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1232,7 +1232,7 @@
         <v>37.66</v>
       </c>
       <c r="O14" t="n">
-        <v>106.27</v>
+        <v>104.44</v>
       </c>
       <c r="P14" t="n">
         <v>102.89</v>
@@ -1246,7 +1246,7 @@
         <v>71.84999999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>59.88000106811523</v>
+        <v>59.84000015258789</v>
       </c>
       <c r="D15" t="n">
         <v>59.7</v>
@@ -1255,7 +1255,7 @@
         <v>11.85</v>
       </c>
       <c r="F15" t="n">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="G15" t="n">
         <v>0.31</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>59.88±0.18</t>
+          <t>59.84±0.18</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1288,7 +1288,7 @@
         <v>36.02</v>
       </c>
       <c r="O15" t="n">
-        <v>110.59</v>
+        <v>108.81</v>
       </c>
       <c r="P15" t="n">
         <v>104.93</v>
@@ -1302,7 +1302,7 @@
         <v>76.89</v>
       </c>
       <c r="C16" t="n">
-        <v>63.20999908447266</v>
+        <v>63.18000030517578</v>
       </c>
       <c r="D16" t="n">
         <v>62.7</v>
@@ -1311,7 +1311,7 @@
         <v>13.89</v>
       </c>
       <c r="F16" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="G16" t="n">
         <v>0.3</v>
@@ -1332,7 +1332,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>63.21±0.18</t>
+          <t>63.18±0.18</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1344,7 +1344,7 @@
         <v>34.21</v>
       </c>
       <c r="O16" t="n">
-        <v>105.76</v>
+        <v>106.91</v>
       </c>
       <c r="P16" t="n">
         <v>106.01</v>
@@ -1358,7 +1358,7 @@
         <v>79.95</v>
       </c>
       <c r="C17" t="n">
-        <v>65.23000335693359</v>
+        <v>65.20999908447266</v>
       </c>
       <c r="D17" t="n">
         <v>64.66</v>
@@ -1367,7 +1367,7 @@
         <v>14.95</v>
       </c>
       <c r="F17" t="n">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="G17" t="n">
         <v>0.42</v>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>65.23±0.22</t>
+          <t>65.21±0.22</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1400,7 +1400,7 @@
         <v>33.52</v>
       </c>
       <c r="O17" t="n">
-        <v>103.32</v>
+        <v>104.07</v>
       </c>
       <c r="P17" t="n">
         <v>100.6</v>
@@ -1414,7 +1414,7 @@
         <v>82.73999999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>67.06999969482422</v>
+        <v>67.05000305175781</v>
       </c>
       <c r="D18" t="n">
         <v>66.69</v>
@@ -1423,7 +1423,7 @@
         <v>15.74</v>
       </c>
       <c r="F18" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="G18" t="n">
         <v>0.41</v>
@@ -1444,7 +1444,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>67.07±0.2</t>
+          <t>67.05±0.2</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1456,7 +1456,7 @@
         <v>33.18</v>
       </c>
       <c r="O18" t="n">
-        <v>110.23</v>
+        <v>110.5</v>
       </c>
       <c r="P18" t="n">
         <v>101.66</v>
@@ -1470,7 +1470,7 @@
         <v>87.11</v>
       </c>
       <c r="C19" t="n">
-        <v>69.88999938964844</v>
+        <v>69.87000274658203</v>
       </c>
       <c r="D19" t="n">
         <v>69.72</v>
@@ -1479,7 +1479,7 @@
         <v>17.11</v>
       </c>
       <c r="F19" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
       <c r="G19" t="n">
         <v>0.38</v>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>69.89±0.22</t>
+          <t>69.87±0.22</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1512,7 +1512,7 @@
         <v>32.54</v>
       </c>
       <c r="O19" t="n">
-        <v>110.94</v>
+        <v>110.35</v>
       </c>
       <c r="P19" t="n">
         <v>102.8</v>
@@ -1526,7 +1526,7 @@
         <v>92.11</v>
       </c>
       <c r="C20" t="n">
-        <v>72.98999786376953</v>
+        <v>72.95999908447266</v>
       </c>
       <c r="D20" t="n">
         <v>72.56</v>
@@ -1535,7 +1535,7 @@
         <v>19.11</v>
       </c>
       <c r="F20" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="G20" t="n">
         <v>0.44</v>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>72.99±0.22</t>
+          <t>72.96±0.22</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1568,7 +1568,7 @@
         <v>31.44</v>
       </c>
       <c r="O20" t="n">
-        <v>110.51</v>
+        <v>110.47</v>
       </c>
       <c r="P20" t="n">
         <v>102.02</v>

</xml_diff>